<commit_message>
add diff and days_ahead
</commit_message>
<xml_diff>
--- a/data/report_df/cn_csi300_open_CSRankNorm_mse_IdentityReweighter.xlsx
+++ b/data/report_df/cn_csi300_open_CSRankNorm_mse_IdentityReweighter.xlsx
@@ -418,7 +418,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.00189</v>
+        <v>0.00076</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -427,10 +427,10 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.00114</v>
+        <v>0.00137</v>
       </c>
       <c r="D3">
-        <v>0.00131</v>
+        <v>0.0012</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -439,16 +439,16 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>0.00071</v>
+        <v>0.0009300000000000001</v>
       </c>
       <c r="D4">
-        <v>0.00095</v>
+        <v>0.00122</v>
       </c>
       <c r="E4">
-        <v>0.00123</v>
+        <v>0.00124</v>
       </c>
       <c r="F4">
-        <v>0.00122</v>
+        <v>0.00096</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -460,16 +460,16 @@
         <v>0.00055</v>
       </c>
       <c r="D5">
-        <v>0.00077</v>
+        <v>0.0012</v>
       </c>
       <c r="E5">
-        <v>0.00119</v>
+        <v>0.00138</v>
       </c>
       <c r="F5">
-        <v>0.00117</v>
+        <v>0.00105</v>
       </c>
       <c r="G5">
-        <v>0.00126</v>
+        <v>0.00106</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -478,19 +478,19 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0.00068</v>
+        <v>0.00052</v>
       </c>
       <c r="D6">
-        <v>0.00079</v>
+        <v>0.00099</v>
       </c>
       <c r="E6">
-        <v>0.00117</v>
+        <v>0.00108</v>
       </c>
       <c r="F6">
-        <v>0.0013</v>
+        <v>0.0012</v>
       </c>
       <c r="G6">
-        <v>0.00123</v>
+        <v>0.00134</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -499,19 +499,19 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>0.0005999999999999999</v>
+        <v>0.00047</v>
       </c>
       <c r="D7">
-        <v>0.00074</v>
+        <v>0.00078</v>
       </c>
       <c r="E7">
-        <v>0.00094</v>
+        <v>0.00095</v>
       </c>
       <c r="F7">
-        <v>0.0012</v>
+        <v>0.00123</v>
       </c>
       <c r="G7">
-        <v>0.00109</v>
+        <v>0.00128</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -522,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.02562</v>
+        <v>0.02363</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -531,10 +531,10 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>0.01784</v>
+        <v>0.01786</v>
       </c>
       <c r="D9">
-        <v>0.01737</v>
+        <v>0.01823</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -543,16 +543,16 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.01331</v>
+        <v>0.01318</v>
       </c>
       <c r="D10">
-        <v>0.01198</v>
+        <v>0.01407</v>
       </c>
       <c r="E10">
-        <v>0.01186</v>
+        <v>0.01347</v>
       </c>
       <c r="F10">
-        <v>0.0118</v>
+        <v>0.01167</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -561,19 +561,19 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <v>0.01087</v>
+        <v>0.01092</v>
       </c>
       <c r="D11">
-        <v>0.01035</v>
+        <v>0.01188</v>
       </c>
       <c r="E11">
-        <v>0.01074</v>
+        <v>0.01165</v>
       </c>
       <c r="F11">
-        <v>0.01022</v>
+        <v>0.01058</v>
       </c>
       <c r="G11">
-        <v>0.01028</v>
+        <v>0.01055</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -582,19 +582,19 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>0.01011</v>
+        <v>0.01029</v>
       </c>
       <c r="D12">
-        <v>0.00962</v>
+        <v>0.0098</v>
       </c>
       <c r="E12">
-        <v>0.00991</v>
+        <v>0.01018</v>
       </c>
       <c r="F12">
-        <v>0.009650000000000001</v>
+        <v>0.01014</v>
       </c>
       <c r="G12">
-        <v>0.009639999999999999</v>
+        <v>0.01018</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -603,19 +603,19 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>0.00915</v>
+        <v>0.009180000000000001</v>
       </c>
       <c r="D13">
-        <v>0.00893</v>
+        <v>0.008750000000000001</v>
       </c>
       <c r="E13">
-        <v>0.00882</v>
+        <v>0.008959999999999999</v>
       </c>
       <c r="F13">
-        <v>0.009209999999999999</v>
+        <v>0.00933</v>
       </c>
       <c r="G13">
-        <v>0.008840000000000001</v>
+        <v>0.00895</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -626,7 +626,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>0.44966</v>
+        <v>0.182</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -635,10 +635,10 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>0.27057</v>
+        <v>0.326</v>
       </c>
       <c r="D15">
-        <v>0.3113</v>
+        <v>0.28496</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -647,16 +647,16 @@
         <v>4</v>
       </c>
       <c r="C16">
-        <v>0.16893</v>
+        <v>0.22128</v>
       </c>
       <c r="D16">
-        <v>0.22646</v>
+        <v>0.29065</v>
       </c>
       <c r="E16">
-        <v>0.29324</v>
+        <v>0.29607</v>
       </c>
       <c r="F16">
-        <v>0.28984</v>
+        <v>0.2287</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -665,19 +665,19 @@
         <v>6</v>
       </c>
       <c r="C17">
-        <v>0.132</v>
+        <v>0.13113</v>
       </c>
       <c r="D17">
-        <v>0.18254</v>
+        <v>0.28495</v>
       </c>
       <c r="E17">
-        <v>0.28251</v>
+        <v>0.32741</v>
       </c>
       <c r="F17">
-        <v>0.27872</v>
+        <v>0.25065</v>
       </c>
       <c r="G17">
-        <v>0.29985</v>
+        <v>0.25212</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -686,19 +686,19 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <v>0.16112</v>
+        <v>0.12361</v>
       </c>
       <c r="D18">
-        <v>0.18841</v>
+        <v>0.23514</v>
       </c>
       <c r="E18">
-        <v>0.27782</v>
+        <v>0.25643</v>
       </c>
       <c r="F18">
-        <v>0.30834</v>
+        <v>0.28555</v>
       </c>
       <c r="G18">
-        <v>0.29202</v>
+        <v>0.31915</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -707,19 +707,19 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <v>0.14387</v>
+        <v>0.11162</v>
       </c>
       <c r="D19">
-        <v>0.17647</v>
+        <v>0.18557</v>
       </c>
       <c r="E19">
-        <v>0.22428</v>
+        <v>0.22607</v>
       </c>
       <c r="F19">
-        <v>0.28503</v>
+        <v>0.29186</v>
       </c>
       <c r="G19">
-        <v>0.25835</v>
+        <v>0.30507</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -730,7 +730,7 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>1.13779</v>
+        <v>0.49935</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -739,10 +739,10 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <v>0.9831299999999999</v>
+        <v>1.1834</v>
       </c>
       <c r="D21">
-        <v>1.16183</v>
+        <v>1.01351</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -751,16 +751,16 @@
         <v>4</v>
       </c>
       <c r="C22">
-        <v>0.82258</v>
+        <v>1.08822</v>
       </c>
       <c r="D22">
-        <v>1.22523</v>
+        <v>1.33925</v>
       </c>
       <c r="E22">
-        <v>1.60306</v>
+        <v>1.42518</v>
       </c>
       <c r="F22">
-        <v>1.59254</v>
+        <v>1.27009</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -769,19 +769,19 @@
         <v>6</v>
       </c>
       <c r="C23">
-        <v>0.78717</v>
+        <v>0.77837</v>
       </c>
       <c r="D23">
-        <v>1.14363</v>
+        <v>1.55526</v>
       </c>
       <c r="E23">
-        <v>1.70529</v>
+        <v>1.82155</v>
       </c>
       <c r="F23">
-        <v>1.76716</v>
+        <v>1.5355</v>
       </c>
       <c r="G23">
-        <v>1.88997</v>
+        <v>1.54896</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -790,19 +790,19 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>1.03252</v>
+        <v>0.7786</v>
       </c>
       <c r="D24">
-        <v>1.26945</v>
+        <v>1.55587</v>
       </c>
       <c r="E24">
-        <v>1.81759</v>
+        <v>1.63301</v>
       </c>
       <c r="F24">
-        <v>2.07139</v>
+        <v>1.82569</v>
       </c>
       <c r="G24">
-        <v>1.96321</v>
+        <v>2.03259</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -811,19 +811,19 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <v>1.0195</v>
+        <v>0.78832</v>
       </c>
       <c r="D25">
-        <v>1.28115</v>
+        <v>1.37433</v>
       </c>
       <c r="E25">
-        <v>1.64852</v>
+        <v>1.63514</v>
       </c>
       <c r="F25">
-        <v>2.00673</v>
+        <v>2.02711</v>
       </c>
       <c r="G25">
-        <v>1.89457</v>
+        <v>2.20827</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -834,7 +834,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>-0.48156</v>
+        <v>-0.53932</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -843,10 +843,10 @@
         <v>2</v>
       </c>
       <c r="C27">
-        <v>-0.39196</v>
+        <v>-0.27228</v>
       </c>
       <c r="D27">
-        <v>-0.33688</v>
+        <v>-0.34336</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -855,16 +855,16 @@
         <v>4</v>
       </c>
       <c r="C28">
-        <v>-0.24669</v>
+        <v>-0.2453</v>
       </c>
       <c r="D28">
-        <v>-0.26726</v>
+        <v>-0.27391</v>
       </c>
       <c r="E28">
-        <v>-0.25008</v>
+        <v>-0.2589</v>
       </c>
       <c r="F28">
-        <v>-0.25001</v>
+        <v>-0.29511</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -873,19 +873,19 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>-0.23145</v>
+        <v>-0.19179</v>
       </c>
       <c r="D29">
-        <v>-0.23539</v>
+        <v>-0.18552</v>
       </c>
       <c r="E29">
-        <v>-0.19741</v>
+        <v>-0.16682</v>
       </c>
       <c r="F29">
-        <v>-0.19188</v>
+        <v>-0.19422</v>
       </c>
       <c r="G29">
-        <v>-0.20431</v>
+        <v>-0.17538</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -894,19 +894,19 @@
         <v>8</v>
       </c>
       <c r="C30">
-        <v>-0.18555</v>
+        <v>-0.21058</v>
       </c>
       <c r="D30">
-        <v>-0.18237</v>
+        <v>-0.18346</v>
       </c>
       <c r="E30">
-        <v>-0.20207</v>
+        <v>-0.1729</v>
       </c>
       <c r="F30">
-        <v>-0.19104</v>
+        <v>-0.116</v>
       </c>
       <c r="G30">
-        <v>-0.19304</v>
+        <v>-0.11739</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -915,19 +915,19 @@
         <v>10</v>
       </c>
       <c r="C31">
-        <v>-0.15646</v>
+        <v>-0.20559</v>
       </c>
       <c r="D31">
-        <v>-0.18971</v>
+        <v>-0.15441</v>
       </c>
       <c r="E31">
-        <v>-0.17222</v>
+        <v>-0.15447</v>
       </c>
       <c r="F31">
-        <v>-0.20407</v>
+        <v>-0.11283</v>
       </c>
       <c r="G31">
-        <v>-0.18703</v>
+        <v>-0.10983</v>
       </c>
     </row>
   </sheetData>
@@ -975,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.00013</v>
+        <v>-0.00084</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -984,10 +984,10 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.00016</v>
+        <v>0.00041</v>
       </c>
       <c r="D3">
-        <v>-0.00014</v>
+        <v>-0.00034</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -996,16 +996,16 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>0.00021</v>
+        <v>0.00044</v>
       </c>
       <c r="D4">
-        <v>4E-05</v>
+        <v>0.00026</v>
       </c>
       <c r="E4">
-        <v>0.00011</v>
+        <v>-5E-05</v>
       </c>
       <c r="F4">
-        <v>6.999999999999999E-05</v>
+        <v>-0.00016</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1014,19 +1014,19 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>0.00022</v>
+        <v>0.00023</v>
       </c>
       <c r="D5">
-        <v>0.00011</v>
+        <v>0.00054</v>
       </c>
       <c r="E5">
-        <v>0.00022</v>
+        <v>0.00042</v>
       </c>
       <c r="F5">
-        <v>0.00011</v>
+        <v>-8.000000000000001E-05</v>
       </c>
       <c r="G5">
-        <v>0.00012</v>
+        <v>-0.00015</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1035,19 +1035,19 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0.00042</v>
+        <v>0.00026</v>
       </c>
       <c r="D6">
-        <v>0.00026</v>
+        <v>0.00046</v>
       </c>
       <c r="E6">
-        <v>0.00041</v>
+        <v>0.00032</v>
       </c>
       <c r="F6">
-        <v>0.00033</v>
+        <v>0.00023</v>
       </c>
       <c r="G6">
-        <v>0.00011</v>
+        <v>0.00021</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1056,19 +1056,19 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>0.00039</v>
+        <v>0.00027</v>
       </c>
       <c r="D7">
-        <v>0.00032</v>
+        <v>0.00036</v>
       </c>
       <c r="E7">
-        <v>0.00032</v>
+        <v>0.00034</v>
       </c>
       <c r="F7">
-        <v>0.00039</v>
+        <v>0.00043</v>
       </c>
       <c r="G7">
-        <v>0.00014</v>
+        <v>0.00036</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1079,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.02568</v>
+        <v>0.02365</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1088,10 +1088,10 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>0.01784</v>
+        <v>0.01786</v>
       </c>
       <c r="D9">
-        <v>0.01741</v>
+        <v>0.01824</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1100,16 +1100,16 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0.01331</v>
+        <v>0.01318</v>
       </c>
       <c r="D10">
-        <v>0.012</v>
+        <v>0.01407</v>
       </c>
       <c r="E10">
-        <v>0.01188</v>
+        <v>0.01347</v>
       </c>
       <c r="F10">
-        <v>0.01183</v>
+        <v>0.01167</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1118,19 +1118,19 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <v>0.01087</v>
+        <v>0.01092</v>
       </c>
       <c r="D11">
-        <v>0.01035</v>
+        <v>0.01188</v>
       </c>
       <c r="E11">
-        <v>0.01074</v>
+        <v>0.01166</v>
       </c>
       <c r="F11">
-        <v>0.01024</v>
+        <v>0.01059</v>
       </c>
       <c r="G11">
-        <v>0.01031</v>
+        <v>0.01056</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1139,19 +1139,19 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>0.01012</v>
+        <v>0.01029</v>
       </c>
       <c r="D12">
-        <v>0.00962</v>
+        <v>0.0098</v>
       </c>
       <c r="E12">
-        <v>0.00991</v>
+        <v>0.01018</v>
       </c>
       <c r="F12">
-        <v>0.009650000000000001</v>
+        <v>0.01014</v>
       </c>
       <c r="G12">
-        <v>0.009650000000000001</v>
+        <v>0.01018</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1160,19 +1160,19 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>0.009140000000000001</v>
+        <v>0.009180000000000001</v>
       </c>
       <c r="D13">
-        <v>0.00893</v>
+        <v>0.008750000000000001</v>
       </c>
       <c r="E13">
-        <v>0.00882</v>
+        <v>0.008959999999999999</v>
       </c>
       <c r="F13">
-        <v>0.009209999999999999</v>
+        <v>0.009339999999999999</v>
       </c>
       <c r="G13">
-        <v>0.00885</v>
+        <v>0.008959999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1183,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>0.03087</v>
+        <v>-0.1997</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1192,10 +1192,10 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>0.03893</v>
+        <v>0.09846000000000001</v>
       </c>
       <c r="D15">
-        <v>-0.03338</v>
+        <v>-0.08185000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1204,16 +1204,16 @@
         <v>4</v>
       </c>
       <c r="C16">
-        <v>0.05077</v>
+        <v>0.10506</v>
       </c>
       <c r="D16">
-        <v>0.009010000000000001</v>
+        <v>0.06136</v>
       </c>
       <c r="E16">
-        <v>0.02687</v>
+        <v>-0.0118</v>
       </c>
       <c r="F16">
-        <v>0.01579</v>
+        <v>-0.03864</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1222,19 +1222,19 @@
         <v>6</v>
       </c>
       <c r="C17">
-        <v>0.05173</v>
+        <v>0.05374</v>
       </c>
       <c r="D17">
-        <v>0.02551</v>
+        <v>0.128</v>
       </c>
       <c r="E17">
-        <v>0.05143</v>
+        <v>0.09909</v>
       </c>
       <c r="F17">
-        <v>0.02534</v>
+        <v>-0.01888</v>
       </c>
       <c r="G17">
-        <v>0.0277</v>
+        <v>-0.03461</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1243,19 +1243,19 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <v>0.09943</v>
+        <v>0.06288000000000001</v>
       </c>
       <c r="D18">
-        <v>0.06157</v>
+        <v>0.11052</v>
       </c>
       <c r="E18">
-        <v>0.09723999999999999</v>
+        <v>0.07653</v>
       </c>
       <c r="F18">
-        <v>0.07746</v>
+        <v>0.05494</v>
       </c>
       <c r="G18">
-        <v>0.0258</v>
+        <v>0.04995</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1264,19 +1264,19 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <v>0.09229999999999999</v>
+        <v>0.06368</v>
       </c>
       <c r="D19">
-        <v>0.07581</v>
+        <v>0.08484</v>
       </c>
       <c r="E19">
-        <v>0.07563</v>
+        <v>0.08172</v>
       </c>
       <c r="F19">
-        <v>0.09378</v>
+        <v>0.1031</v>
       </c>
       <c r="G19">
-        <v>0.03399</v>
+        <v>0.08464000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1287,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>0.07792</v>
+        <v>-0.5472399999999999</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1296,10 +1296,10 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <v>0.14143</v>
+        <v>0.35727</v>
       </c>
       <c r="D21">
-        <v>-0.12426</v>
+        <v>-0.29081</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1308,16 +1308,16 @@
         <v>4</v>
       </c>
       <c r="C22">
-        <v>0.24723</v>
+        <v>0.5166500000000001</v>
       </c>
       <c r="D22">
-        <v>0.04867</v>
+        <v>0.28267</v>
       </c>
       <c r="E22">
-        <v>0.14655</v>
+        <v>-0.0568</v>
       </c>
       <c r="F22">
-        <v>0.08653</v>
+        <v>-0.21463</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1326,19 +1326,19 @@
         <v>6</v>
       </c>
       <c r="C23">
-        <v>0.30838</v>
+        <v>0.319</v>
       </c>
       <c r="D23">
-        <v>0.15975</v>
+        <v>0.6986</v>
       </c>
       <c r="E23">
-        <v>0.31038</v>
+        <v>0.551</v>
       </c>
       <c r="F23">
-        <v>0.16034</v>
+        <v>-0.11558</v>
       </c>
       <c r="G23">
-        <v>0.17421</v>
+        <v>-0.21245</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1347,19 +1347,19 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>0.63712</v>
+        <v>0.39612</v>
       </c>
       <c r="D24">
-        <v>0.41486</v>
+        <v>0.73123</v>
       </c>
       <c r="E24">
-        <v>0.63614</v>
+        <v>0.4872</v>
       </c>
       <c r="F24">
-        <v>0.52011</v>
+        <v>0.35105</v>
       </c>
       <c r="G24">
-        <v>0.17325</v>
+        <v>0.31794</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1368,19 +1368,19 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <v>0.65429</v>
+        <v>0.44974</v>
       </c>
       <c r="D25">
-        <v>0.55036</v>
+        <v>0.62818</v>
       </c>
       <c r="E25">
-        <v>0.55581</v>
+        <v>0.59088</v>
       </c>
       <c r="F25">
-        <v>0.66011</v>
+        <v>0.71591</v>
       </c>
       <c r="G25">
-        <v>0.24903</v>
+        <v>0.61254</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1391,7 +1391,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>-0.8504</v>
+        <v>-1.45429</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1400,10 +1400,10 @@
         <v>2</v>
       </c>
       <c r="C27">
-        <v>-0.67395</v>
+        <v>-0.35905</v>
       </c>
       <c r="D27">
-        <v>-0.83391</v>
+        <v>-0.91329</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1412,16 +1412,16 @@
         <v>4</v>
       </c>
       <c r="C28">
-        <v>-0.32364</v>
+        <v>-0.29043</v>
       </c>
       <c r="D28">
-        <v>-0.51525</v>
+        <v>-0.46343</v>
       </c>
       <c r="E28">
-        <v>-0.61064</v>
+        <v>-0.64085</v>
       </c>
       <c r="F28">
-        <v>-0.60516</v>
+        <v>-0.63205</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1430,19 +1430,19 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>-0.26276</v>
+        <v>-0.23869</v>
       </c>
       <c r="D29">
-        <v>-0.35436</v>
+        <v>-0.29182</v>
       </c>
       <c r="E29">
-        <v>-0.31988</v>
+        <v>-0.35236</v>
       </c>
       <c r="F29">
-        <v>-0.50676</v>
+        <v>-0.47483</v>
       </c>
       <c r="G29">
-        <v>-0.44619</v>
+        <v>-0.49182</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1451,19 +1451,19 @@
         <v>8</v>
       </c>
       <c r="C30">
-        <v>-0.20994</v>
+        <v>-0.23253</v>
       </c>
       <c r="D30">
-        <v>-0.25622</v>
+        <v>-0.23223</v>
       </c>
       <c r="E30">
-        <v>-0.23152</v>
+        <v>-0.30104</v>
       </c>
       <c r="F30">
-        <v>-0.26634</v>
+        <v>-0.2392</v>
       </c>
       <c r="G30">
-        <v>-0.38412</v>
+        <v>-0.26926</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1472,19 +1472,19 @@
         <v>10</v>
       </c>
       <c r="C31">
-        <v>-0.17773</v>
+        <v>-0.22346</v>
       </c>
       <c r="D31">
-        <v>-0.20467</v>
+        <v>-0.19504</v>
       </c>
       <c r="E31">
-        <v>-0.19844</v>
+        <v>-0.2355</v>
       </c>
       <c r="F31">
-        <v>-0.27129</v>
+        <v>-0.18331</v>
       </c>
       <c r="G31">
-        <v>-0.33907</v>
+        <v>-0.18295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>